<commit_message>
Update README and projects data
</commit_message>
<xml_diff>
--- a/data/projects.xlsx
+++ b/data/projects.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -742,6 +742,46 @@
       </c>
       <c r="D16" t="n">
         <v>14</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>route</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>route</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>🧭</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>桌面工具</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>桌面工具</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>🖥️</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -755,7 +795,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H68"/>
+  <dimension ref="A1:H80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -973,22 +1013,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>nanobot</t>
+          <t>ten-framework</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>nanobot</t>
+          <t>TEN Framework</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Lightweight AI agent framework and tooling</t>
+          <t>Open-source framework for building real-time multimodal AI agents</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://github.com/HKUDS/nanobot</t>
+          <t>https://github.com/TEN-framework/ten-framework</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -998,7 +1038,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-81fa-ad3e-f6cb074f1dc7</t>
+          <t>300d0e79-ce27-814b-91a7-f9ad894faa5c</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -1013,32 +1053,24 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ten-framework</t>
+          <t>camel</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>TEN Framework</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Open-source framework for building real-time multimodal AI agents</t>
-        </is>
-      </c>
+          <t>camel</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://github.com/TEN-framework/ten-framework</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>ai, agents, framework</t>
-        </is>
-      </c>
+          <t>https://github.com/camel-ai/camel</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-814b-91a7-f9ad894faa5c</t>
+          <t>304d0e79-ce27-81b8-82c0-d3a43da7e040</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -1048,41 +1080,33 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>memory</t>
+          <t>ai-agents</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>memoryos</t>
+          <t>agno</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MemoryOS</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Persistent memory operating layer for AI agents</t>
-        </is>
-      </c>
+          <t>agno</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://github.com/BAI-LAB/MemoryOS</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>memory, agents, ai</t>
-        </is>
-      </c>
+          <t>https://github.com/agno-agi/agno</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-814e-908f-e19f0bf369a3</t>
+          <t>304d0e79-ce27-819f-844d-c6ec6b6af5ed</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
@@ -1093,36 +1117,36 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>mem0</t>
+          <t>memoryos</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>mem0</t>
+          <t>MemoryOS</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Memory layer for personalized AI applications and agents</t>
+          <t>Persistent memory operating layer for AI agents</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://github.com/mem0ai/mem0</t>
+          <t>https://github.com/BAI-LAB/MemoryOS</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>memory, ai, personalization</t>
+          <t>memory, agents, ai</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-81c1-9461-dbe40bf2195e</t>
+          <t>300d0e79-ce27-814e-908f-e19f0bf369a3</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1133,116 +1157,108 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>letta</t>
+          <t>mem0</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Letta</t>
+          <t>mem0</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Stateful agent framework with long-term memory</t>
+          <t>Memory layer for personalized AI applications and agents</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://github.com/letta-ai/letta</t>
+          <t>https://github.com/mem0ai/mem0</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>agents, memory, llm</t>
+          <t>memory, ai, personalization</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-81a0-a418-e7690e8f1176</t>
+          <t>300d0e79-ce27-81c1-9461-dbe40bf2195e</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>data-workflow</t>
+          <t>memory</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>deepwiki-mcp</t>
+          <t>letta</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>deepwiki-mcp</t>
+          <t>Letta</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>MCP server integration for DeepWiki-style knowledge workflows</t>
+          <t>Stateful agent framework with long-term memory</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://github.com/regenrek/deepwiki-mcp</t>
+          <t>https://github.com/letta-ai/letta</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>mcp, knowledge, workflow</t>
+          <t>agents, memory, llm</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8166-93f0-d10c442fa92b</t>
+          <t>300d0e79-ce27-81a0-a418-e7690e8f1176</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>data-workflow</t>
+          <t>memory</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>dataflow</t>
+          <t>evermemos</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>DataFlow</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Open framework for data-centric AI workflows</t>
-        </is>
-      </c>
+          <t>EverMemOS</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://github.com/OpenDCAI/DataFlow</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>data, workflow, ai</t>
-        </is>
-      </c>
+          <t>https://github.com/EverMind-AI/EverMemOS</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8151-b103-f48d1f14781f</t>
+          <t>304d0e79-ce27-81a3-bbf0-c7fd99e89361</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
@@ -1253,36 +1269,36 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>dataflow-agent</t>
+          <t>deepwiki-mcp</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>DataFlow-Agent</t>
+          <t>deepwiki-mcp</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Agent extension for DataFlow workflow orchestration</t>
+          <t>MCP server integration for DeepWiki-style knowledge workflows</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://github.com/OpenDCAI/DataFlow-Agent</t>
+          <t>https://github.com/regenrek/deepwiki-mcp</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>agents, workflow, data</t>
+          <t>mcp, knowledge, workflow</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-817f-9b57-cec9f1afe155</t>
+          <t>300d0e79-ce27-8166-93f0-d10c442fa92b</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1293,36 +1309,36 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ragflow</t>
+          <t>dataflow</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>RAGFlow</t>
+          <t>DataFlow</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Open-source RAG workflow platform for document QA and knowledge apps</t>
+          <t>Open framework for data-centric AI workflows</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://github.com/infiniflow/ragflow</t>
+          <t>https://github.com/OpenDCAI/DataFlow</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>rag, workflow, knowledge-base</t>
+          <t>data, workflow, ai</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8102-a9cd-dbc60b3d4f89</t>
+          <t>300d0e79-ce27-8151-b103-f48d1f14781f</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -1333,116 +1349,116 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>dify</t>
+          <t>dataflow-agent</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Dify</t>
+          <t>DataFlow-Agent</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>LLM application development platform with workflow orchestration</t>
+          <t>Agent extension for DataFlow workflow orchestration</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://github.com/langgenius/dify</t>
+          <t>https://github.com/OpenDCAI/DataFlow-Agent</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>llm, workflow, ai-app</t>
+          <t>agents, workflow, data</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8114-9c42-fbb7a6321c71</t>
+          <t>300d0e79-ce27-817f-9b57-cec9f1afe155</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>llm-training</t>
+          <t>data-workflow</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>minimind</t>
+          <t>ragflow</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MiniMind</t>
+          <t>RAGFlow</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Lightweight minimal LLM training and inference project</t>
+          <t>Open-source RAG workflow platform for document QA and knowledge apps</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://github.com/jingyaogong/minimind</t>
+          <t>https://github.com/infiniflow/ragflow</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>llm, training, inference</t>
+          <t>rag, workflow, knowledge-base</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-810e-8d34-c098f8ee421f</t>
+          <t>300d0e79-ce27-8102-a9cd-dbc60b3d4f89</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>llm-training</t>
+          <t>data-workflow</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ms-swift</t>
+          <t>dify</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ms-swift</t>
+          <t>Dify</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>ModelScope framework for LLM training, fine-tuning, and deployment</t>
+          <t>LLM application development platform with workflow orchestration</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://github.com/modelscope/ms-swift</t>
+          <t>https://github.com/langgenius/dify</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>llm, finetuning, deployment</t>
+          <t>llm, workflow, ai-app</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-81be-a764-fded4211ff1b</t>
+          <t>300d0e79-ce27-8114-9c42-fbb7a6321c71</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -1453,116 +1469,116 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>llamafactory</t>
+          <t>minimind</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>LLaMA-Factory</t>
+          <t>MiniMind</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Unified and efficient fine-tuning framework for large language models</t>
+          <t>Lightweight minimal LLM training and inference project</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://github.com/hiyouga/LlamaFactory</t>
+          <t>https://github.com/jingyaogong/minimind</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>llm, finetuning, training</t>
+          <t>llm, training, inference</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8102-ba22-ef1f41de00a9</t>
+          <t>300d0e79-ce27-810e-8d34-c098f8ee421f</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>agent-apps</t>
+          <t>llm-training</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>trainpptagent</t>
+          <t>ms-swift</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>TrainPPTAgent</t>
+          <t>ms-swift</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Agent for generating and training presentation workflows</t>
+          <t>ModelScope framework for LLM training, fine-tuning, and deployment</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://github.com/johnson7788/TrainPPTAgent</t>
+          <t>https://github.com/modelscope/ms-swift</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>agent, ppt, automation</t>
+          <t>llm, finetuning, deployment</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-81bf-a155-d9743510696f</t>
+          <t>300d0e79-ce27-81be-a764-fded4211ff1b</t>
         </is>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>agent-apps</t>
+          <t>llm-training</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ag-ui</t>
+          <t>llamafactory</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ag-ui</t>
+          <t>LLaMA-Factory</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Protocol for interoperable agent-user interface communication</t>
+          <t>Unified and efficient fine-tuning framework for large language models</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://github.com/ag-ui-protocol/ag-ui</t>
+          <t>https://github.com/hiyouga/LlamaFactory</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>protocol, ui, agents</t>
+          <t>llm, finetuning, training</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8183-8ebd-cd74a1fa3c34</t>
+          <t>300d0e79-ce27-8102-ba22-ef1f41de00a9</t>
         </is>
       </c>
       <c r="H20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -1573,152 +1589,152 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>open-avatar-chat</t>
+          <t>trainpptagent</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>OpenAvatarChat</t>
+          <t>TrainPPTAgent</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Open-source avatar chat application for human-AI interaction</t>
+          <t>Agent for generating and training presentation workflows</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://github.com/HumanAIGC-Engineering/OpenAvatarChat</t>
+          <t>https://github.com/johnson7788/TrainPPTAgent</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>avatar, chat, ai</t>
+          <t>agent, ppt, automation</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-810a-b01d-f96cf39807ce</t>
+          <t>300d0e79-ce27-81bf-a155-d9743510696f</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>practice-projects</t>
+          <t>agent-apps</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>asr-llm-tts</t>
+          <t>ag-ui</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>asr-llm-tts</t>
+          <t>ag-ui</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Practice project integrating ASR, LLM, and TTS pipeline</t>
+          <t>Protocol for interoperable agent-user interface communication</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://github.com/muggle-stack/asr-llm-tts</t>
+          <t>https://github.com/ag-ui-protocol/ag-ui</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>asr, llm, tts</t>
+          <t>protocol, ui, agents</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-817d-8528-f06a93916e38</t>
+          <t>300d0e79-ce27-8183-8ebd-cd74a1fa3c34</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>practice-projects</t>
+          <t>agent-apps</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>sdyj-multi-agents</t>
+          <t>open-avatar-chat</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>SDYJ_Multi_Agents</t>
+          <t>OpenAvatarChat</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Practice project for building multi-agent collaboration workflows</t>
+          <t>Open-source avatar chat application for human-AI interaction</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://github.com/hwfengcs/SDYJ_Multi_Agents</t>
+          <t>https://github.com/HumanAIGC-Engineering/OpenAvatarChat</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>multi-agent, practice, workflow</t>
+          <t>avatar, chat, ai</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8127-a02c-fb251943f2e2</t>
+          <t>300d0e79-ce27-810a-b01d-f96cf39807ce</t>
         </is>
       </c>
       <c r="H23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>frontend-components</t>
+          <t>practice-projects</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>shadcn-ui</t>
+          <t>asr-llm-tts</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>shadcn-ui</t>
+          <t>asr-llm-tts</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Popular frontend component system and UI building blocks</t>
+          <t>Practice project integrating ASR, LLM, and TTS pipeline</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://github.com/shadcn-ui/ui</t>
+          <t>https://github.com/muggle-stack/asr-llm-tts</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>frontend, components, ui</t>
+          <t>asr, llm, tts</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8123-9579-dc538213105f</t>
+          <t>300d0e79-ce27-817d-8528-f06a93916e38</t>
         </is>
       </c>
       <c r="H24" t="n">
@@ -1728,37 +1744,37 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>frontend-components</t>
+          <t>practice-projects</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>superdesign</t>
+          <t>sdyj-multi-agents</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>superdesign</t>
+          <t>SDYJ_Multi_Agents</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Frontend component library and design system utilities</t>
+          <t>Practice project for building multi-agent collaboration workflows</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>https://github.com/superdesigndev/superdesign</t>
+          <t>https://github.com/hwfengcs/SDYJ_Multi_Agents</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>frontend, components, design-system</t>
+          <t>multi-agent, practice, workflow</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-819b-9eee-d4402848d2ea</t>
+          <t>300d0e79-ce27-8127-a02c-fb251943f2e2</t>
         </is>
       </c>
       <c r="H25" t="n">
@@ -1768,37 +1784,37 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ai-trader</t>
+          <t>frontend-components</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ai-trade-game</t>
+          <t>shadcn-ui</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>AITradeGame</t>
+          <t>shadcn-ui</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>AI-powered trading simulation and strategy game project</t>
+          <t>Popular frontend component system and UI building blocks</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>https://github.com/chadyi/AITradeGame</t>
+          <t>https://github.com/shadcn-ui/ui</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>ai, trading, simulation</t>
+          <t>frontend, components, ui</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-811e-9d25-f7e0d58e192a</t>
+          <t>300d0e79-ce27-8123-9579-dc538213105f</t>
         </is>
       </c>
       <c r="H26" t="n">
@@ -1808,37 +1824,37 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>ai-trader</t>
+          <t>frontend-components</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ai-trader-hkuds</t>
+          <t>superdesign</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>AI-Trader</t>
+          <t>superdesign</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>AI-driven trader framework and research project</t>
+          <t>Frontend component library and design system utilities</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>https://github.com/HKUDS/AI-Trader</t>
+          <t>https://github.com/superdesigndev/superdesign</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>ai, trader, finance</t>
+          <t>frontend, components, design-system</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8133-af38-db68440ac074</t>
+          <t>300d0e79-ce27-819b-9eee-d4402848d2ea</t>
         </is>
       </c>
       <c r="H27" t="n">
@@ -1848,37 +1864,29 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>ai-trader</t>
+          <t>frontend-components</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ai-trading-agent-hkirat</t>
+          <t>chainlit</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ai-trading-agent</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Agent-based automated trading workflow project</t>
-        </is>
-      </c>
+          <t>chainlit</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr">
         <is>
-          <t>https://github.com/hkirat/ai-trading-agent</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>ai, agent, trading</t>
-        </is>
-      </c>
+          <t>https://github.com/Chainlit/chainlit</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-817b-99e5-c488c6215599</t>
+          <t>304d0e79-ce27-8169-9bd9-e82ebc787796</t>
         </is>
       </c>
       <c r="H28" t="n">
@@ -1893,36 +1901,36 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>finance-trading-ai-agents-mcp</t>
+          <t>ai-trade-game</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>finance-trading-ai-agents-mcp</t>
+          <t>AITradeGame</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Finance trading AI agents with MCP integration</t>
+          <t>AI-powered trading simulation and strategy game project</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>https://github.com/aitrados/finance-trading-ai-agents-mcp</t>
+          <t>https://github.com/chadyi/AITradeGame</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>finance, trading, mcp</t>
+          <t>ai, trading, simulation</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8102-8d81-f6c9607a478f</t>
+          <t>300d0e79-ce27-811e-9d25-f7e0d58e192a</t>
         </is>
       </c>
       <c r="H29" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1933,36 +1941,36 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>tradingagents-cn</t>
+          <t>ai-trader-hkuds</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>TradingAgents-CN</t>
+          <t>AI-Trader</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Chinese adaptation of multi-agent trading system</t>
+          <t>AI-driven trader framework and research project</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>https://github.com/hsliuping/TradingAgents-CN</t>
+          <t>https://github.com/HKUDS/AI-Trader</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>trading, agents, cn</t>
+          <t>ai, trader, finance</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-81a8-bdd4-e3598fa5538a</t>
+          <t>300d0e79-ce27-8133-af38-db68440ac074</t>
         </is>
       </c>
       <c r="H30" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -1973,36 +1981,36 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>tradingagents</t>
+          <t>ai-trading-agent-hkirat</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>TradingAgents</t>
+          <t>ai-trading-agent</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Multi-agent architecture for quantitative trading research</t>
+          <t>Agent-based automated trading workflow project</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>https://github.com/TauricResearch/TradingAgents</t>
+          <t>https://github.com/hkirat/ai-trading-agent</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>trading, agents, quant</t>
+          <t>ai, agent, trading</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8166-b8ee-fe7036896318</t>
+          <t>300d0e79-ce27-817b-99e5-c488c6215599</t>
         </is>
       </c>
       <c r="H31" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -2013,156 +2021,156 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>stock-quant</t>
+          <t>finance-trading-ai-agents-mcp</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>stock-quant</t>
+          <t>finance-trading-ai-agents-mcp</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Stock quantitative analysis and trading strategy toolkit</t>
+          <t>Finance trading AI agents with MCP integration</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>https://github.com/zhaoxusun/stock-quant</t>
+          <t>https://github.com/aitrados/finance-trading-ai-agents-mcp</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>stock, quant, trading</t>
+          <t>finance, trading, mcp</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-81d1-a1b1-daa6dff5e4a3</t>
+          <t>300d0e79-ce27-8102-8d81-f6c9607a478f</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>books</t>
+          <t>ai-trader</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>reasoning-from-scratch</t>
+          <t>tradingagents-cn</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>reasoning-from-scratch</t>
+          <t>TradingAgents-CN</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Book project: build and understand LLM reasoning from scratch</t>
+          <t>Chinese adaptation of multi-agent trading system</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>https://github.com/rasbt/reasoning-from-scratch</t>
+          <t>https://github.com/hsliuping/TradingAgents-CN</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>book, reasoning, llm</t>
+          <t>trading, agents, cn</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8154-b542-ca7aa6812d8e</t>
+          <t>300d0e79-ce27-81a8-bdd4-e3598fa5538a</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>books</t>
+          <t>ai-trader</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>reasoning-from-scratch-cn</t>
+          <t>tradingagents</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>reasoning-from-scratch-CN</t>
+          <t>TradingAgents</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Chinese edition of reasoning-from-scratch book project</t>
+          <t>Multi-agent architecture for quantitative trading research</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>https://github.com/MLNLP-World/reasoning-from-scratch-CN</t>
+          <t>https://github.com/TauricResearch/TradingAgents</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>book, reasoning, cn</t>
+          <t>trading, agents, quant</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-81a7-b368-d9d9ade91e23</t>
+          <t>300d0e79-ce27-8166-b8ee-fe7036896318</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>books</t>
+          <t>ai-trader</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>llms-from-scratch-cn</t>
+          <t>stock-quant</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>LLMs-from-scratch-CN</t>
+          <t>stock-quant</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Chinese edition of LLMs-from-scratch book project</t>
+          <t>Stock quantitative analysis and trading strategy toolkit</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>https://github.com/MLNLP-World/LLMs-from-scratch-CN</t>
+          <t>https://github.com/zhaoxusun/stock-quant</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>book, llm, cn</t>
+          <t>stock, quant, trading</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-814e-8a7b-f7530ac092ab</t>
+          <t>300d0e79-ce27-81d1-a1b1-daa6dff5e4a3</t>
         </is>
       </c>
       <c r="H35" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36">
@@ -2173,36 +2181,36 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>llms-from-scratch</t>
+          <t>reasoning-from-scratch</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>LLMs-from-scratch</t>
+          <t>reasoning-from-scratch</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Book project: learn large language models from scratch</t>
+          <t>Book project: build and understand LLM reasoning from scratch</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>https://github.com/rasbt/LLMs-from-scratch</t>
+          <t>https://github.com/rasbt/reasoning-from-scratch</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>book, llm, from-scratch</t>
+          <t>book, reasoning, llm</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8185-8125-c45f0fda2ba1</t>
+          <t>300d0e79-ce27-8154-b542-ca7aa6812d8e</t>
         </is>
       </c>
       <c r="H36" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -2213,36 +2221,36 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>vibe-coding-cn</t>
+          <t>reasoning-from-scratch-cn</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>vibe-coding-cn</t>
+          <t>reasoning-from-scratch-CN</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Chinese learning material repository for vibe coding</t>
+          <t>Chinese edition of reasoning-from-scratch book project</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>https://github.com/2025Emma/vibe-coding-cn</t>
+          <t>https://github.com/MLNLP-World/reasoning-from-scratch-CN</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>book, coding, cn</t>
+          <t>book, reasoning, cn</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8164-b8b0-d450b2c7a814</t>
+          <t>300d0e79-ce27-81a7-b368-d9d9ade91e23</t>
         </is>
       </c>
       <c r="H37" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -2253,36 +2261,36 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>hello-agents</t>
+          <t>llms-from-scratch-cn</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Hello-Agents</t>
+          <t>LLMs-from-scratch-CN</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Educational book-style project for getting started with AI agents</t>
+          <t>Chinese edition of LLMs-from-scratch book project</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>https://github.com/datawhalechina/Hello-Agents</t>
+          <t>https://github.com/MLNLP-World/LLMs-from-scratch-CN</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>book, agents, education</t>
+          <t>book, llm, cn</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8162-85a3-cc5174146797</t>
+          <t>300d0e79-ce27-814e-8a7b-f7530ac092ab</t>
         </is>
       </c>
       <c r="H38" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -2293,36 +2301,36 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>intro-llm-code</t>
+          <t>llms-from-scratch</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>intro-llm-code</t>
+          <t>LLMs-from-scratch</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Code companion repository for introductory LLM learning materials</t>
+          <t>Book project: learn large language models from scratch</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>https://github.com/intro-llm/intro-llm-code</t>
+          <t>https://github.com/rasbt/LLMs-from-scratch</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>book, llm, education</t>
+          <t>book, llm, from-scratch</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-81c0-b736-f258305cb36e</t>
+          <t>300d0e79-ce27-8185-8125-c45f0fda2ba1</t>
         </is>
       </c>
       <c r="H39" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40">
@@ -2333,36 +2341,36 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>vibe-vibe</t>
+          <t>vibe-coding-cn</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>vibe-vibe</t>
+          <t>vibe-coding-cn</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Book-style repository on vibe coding practices and workflows</t>
+          <t>Chinese learning material repository for vibe coding</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>https://github.com/datawhalechina/vibe-vibe</t>
+          <t>https://github.com/2025Emma/vibe-coding-cn</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>book, coding, education</t>
+          <t>book, coding, cn</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>301d0e79-ce27-8180-9484-d668388e7a68</t>
+          <t>300d0e79-ce27-8164-b8b0-d450b2c7a814</t>
         </is>
       </c>
       <c r="H40" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41">
@@ -2373,192 +2381,192 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>easy-rl</t>
+          <t>hello-agents</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>easy-rl</t>
+          <t>Hello-Agents</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Educational reinforcement learning repository with book-style tutorials</t>
+          <t>Educational book-style project for getting started with AI agents</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>https://github.com/datawhalechina/easy-rl</t>
+          <t>https://github.com/datawhalechina/Hello-Agents</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>book, rl, education</t>
+          <t>book, agents, education</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-81c2-a134-d03854ae2a00</t>
+          <t>300d0e79-ce27-8162-85a3-cc5174146797</t>
         </is>
       </c>
       <c r="H41" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>pdf-translation</t>
+          <t>books</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>zotero-pdf2zh</t>
+          <t>intro-llm-code</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>zotero-pdf2zh</t>
+          <t>intro-llm-code</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Translate PDF papers to Chinese with Zotero integration</t>
+          <t>Code companion repository for introductory LLM learning materials</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>https://github.com/guaguastandup/zotero-pdf2zh</t>
+          <t>https://github.com/intro-llm/intro-llm-code</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>pdf, translation, zotero</t>
+          <t>book, llm, education</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-81fe-914d-fe62005b026c</t>
+          <t>300d0e79-ce27-81c0-b736-f258305cb36e</t>
         </is>
       </c>
       <c r="H42" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>pdf-translation</t>
+          <t>books</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>babeldoc</t>
+          <t>vibe-vibe</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>BabelDOC</t>
+          <t>vibe-vibe</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>PDF translation and multilingual document processing toolkit</t>
+          <t>Book-style repository on vibe coding practices and workflows</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>https://github.com/funstory-ai/BabelDOC</t>
+          <t>https://github.com/datawhalechina/vibe-vibe</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>pdf, translation, multilingual</t>
+          <t>book, coding, education</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8169-9363-d2844ae62b54</t>
+          <t>304d0e79-ce27-819a-bba8-f64f159e7cff</t>
         </is>
       </c>
       <c r="H43" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>pdf-translation</t>
+          <t>books</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>pdf-math-translate</t>
+          <t>easy-rl</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>PDFMathTranslate</t>
+          <t>easy-rl</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Translate mathematical and scientific PDF content with structure awareness</t>
+          <t>Educational reinforcement learning repository with book-style tutorials</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>https://github.com/PDFMathTranslate/PDFMathTranslate</t>
+          <t>https://github.com/datawhalechina/easy-rl</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>pdf, translation, math</t>
+          <t>book, rl, education</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8128-8662-cff46037c483</t>
+          <t>300d0e79-ce27-81c2-a134-d03854ae2a00</t>
         </is>
       </c>
       <c r="H44" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>pdf-parsing</t>
+          <t>pdf-translation</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>mineru</t>
+          <t>zotero-pdf2zh</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>MinerU</t>
+          <t>zotero-pdf2zh</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Open-source toolkit for PDF parsing and document structure extraction</t>
+          <t>Translate PDF papers to Chinese with Zotero integration</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>https://github.com/opendatalab/MinerU</t>
+          <t>https://github.com/guaguastandup/zotero-pdf2zh</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>pdf, parsing, document-ai</t>
+          <t>pdf, translation, zotero</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8165-825e-f7f89beb878e</t>
+          <t>300d0e79-ce27-81fe-914d-fe62005b026c</t>
         </is>
       </c>
       <c r="H45" t="n">
@@ -2568,37 +2576,37 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>pdf-parsing</t>
+          <t>pdf-translation</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>paddleocr</t>
+          <t>babeldoc</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>PaddleOCR</t>
+          <t>BabelDOC</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>OCR toolkit for document parsing and text extraction</t>
+          <t>PDF translation and multilingual document processing toolkit</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>https://github.com/PaddlePaddle/PaddleOCR</t>
+          <t>https://github.com/funstory-ai/BabelDOC</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>ocr, pdf, document-ai</t>
+          <t>pdf, translation, multilingual</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-819e-94ef-e76e2723bf6a</t>
+          <t>300d0e79-ce27-8169-9363-d2844ae62b54</t>
         </is>
       </c>
       <c r="H46" t="n">
@@ -2608,37 +2616,37 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>pdf-parsing</t>
+          <t>pdf-translation</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>docling</t>
+          <t>pdf-math-translate</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>docling</t>
+          <t>PDFMathTranslate</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Toolkit for document understanding and PDF parsing workflows</t>
+          <t>Translate mathematical and scientific PDF content with structure awareness</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>https://github.com/DS4SD/docling</t>
+          <t>https://github.com/PDFMathTranslate/PDFMathTranslate</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>pdf, parsing, document-ai</t>
+          <t>pdf, translation, math</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8165-8434-cf340bbfd01c</t>
+          <t>300d0e79-ce27-8128-8662-cff46037c483</t>
         </is>
       </c>
       <c r="H47" t="n">
@@ -2653,36 +2661,36 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>open-parse</t>
+          <t>mineru</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>open-parse</t>
+          <t>MinerU</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Open-source parser for extracting structured content from documents</t>
+          <t>Open-source toolkit for PDF parsing and document structure extraction</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>https://github.com/Filimoa/open-parse</t>
+          <t>https://github.com/opendatalab/MinerU</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>pdf, parsing, extraction</t>
+          <t>pdf, parsing, document-ai</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8175-a1b4-d97a7f5844a0</t>
+          <t>300d0e79-ce27-8165-825e-f7f89beb878e</t>
         </is>
       </c>
       <c r="H48" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -2693,192 +2701,192 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>pdf-extract-kit</t>
+          <t>paddleocr</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>PDF-Extract-Kit</t>
+          <t>PaddleOCR</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Toolkit for extracting structured information from PDF documents</t>
+          <t>OCR toolkit for document parsing and text extraction</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>https://github.com/opendatalab/PDF-Extract-Kit</t>
+          <t>https://github.com/PaddlePaddle/PaddleOCR</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>pdf, extraction, document-ai</t>
+          <t>ocr, pdf, document-ai</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8171-8241-ef7ee2ba34b1</t>
+          <t>300d0e79-ce27-819e-94ef-e76e2723bf6a</t>
         </is>
       </c>
       <c r="H49" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>inference-frameworks</t>
+          <t>pdf-parsing</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>vllm</t>
+          <t>docling</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>vLLM</t>
+          <t>docling</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>High-throughput and memory-efficient LLM inference and serving engine</t>
+          <t>Toolkit for document understanding and PDF parsing workflows</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>https://github.com/vllm-project/vllm</t>
+          <t>https://github.com/DS4SD/docling</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>inference, serving, llm</t>
+          <t>pdf, parsing, document-ai</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-813a-9568-d1cfc9e7790e</t>
+          <t>300d0e79-ce27-8165-8434-cf340bbfd01c</t>
         </is>
       </c>
       <c r="H50" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>inference-frameworks</t>
+          <t>pdf-parsing</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>sglang</t>
+          <t>open-parse</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>SGLang</t>
+          <t>open-parse</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Fast LLM serving framework with structured generation runtime</t>
+          <t>Open-source parser for extracting structured content from documents</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>https://github.com/sgl-project/sglang</t>
+          <t>https://github.com/Filimoa/open-parse</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>inference, serving, runtime</t>
+          <t>pdf, parsing, extraction</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-81dc-adf3-c2ac130f7daf</t>
+          <t>300d0e79-ce27-8175-a1b4-d97a7f5844a0</t>
         </is>
       </c>
       <c r="H51" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>inference-frameworks</t>
+          <t>pdf-parsing</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>llama-cpp</t>
+          <t>pdf-extract-kit</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>llama.cpp</t>
+          <t>PDF-Extract-Kit</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>C/C++ inference runtime for LLMs with efficient local deployment</t>
+          <t>Toolkit for extracting structured information from PDF documents</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>https://github.com/ggml-org/llama.cpp</t>
+          <t>https://github.com/opendatalab/PDF-Extract-Kit</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>inference, ggml, local-llm</t>
+          <t>pdf, extraction, document-ai</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-810a-a73f-f448ec025433</t>
+          <t>300d0e79-ce27-8171-8241-ef7ee2ba34b1</t>
         </is>
       </c>
       <c r="H52" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>tools</t>
+          <t>inference-frameworks</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>aionui</t>
+          <t>vllm</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>AionUi</t>
+          <t>vLLM</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>AI productivity UI toolset and utility platform</t>
+          <t>High-throughput and memory-efficient LLM inference and serving engine</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>https://github.com/iOfficeAI/AionUi</t>
+          <t>https://github.com/vllm-project/vllm</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>tool, ui, productivity</t>
+          <t>inference, serving, llm</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-81cf-b14e-c7dcf8b06178</t>
+          <t>300d0e79-ce27-813a-9568-d1cfc9e7790e</t>
         </is>
       </c>
       <c r="H53" t="n">
@@ -2888,37 +2896,37 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>tools</t>
+          <t>inference-frameworks</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>pastemd</t>
+          <t>sglang</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>PasteMD</t>
+          <t>SGLang</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Tool for converting and managing pasted content into Markdown</t>
+          <t>Fast LLM serving framework with structured generation runtime</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>https://github.com/RICHQAQ/PasteMD</t>
+          <t>https://github.com/sgl-project/sglang</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>tool, markdown, productivity</t>
+          <t>inference, serving, runtime</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8148-8215-d41868298788</t>
+          <t>300d0e79-ce27-81dc-adf3-c2ac130f7daf</t>
         </is>
       </c>
       <c r="H54" t="n">
@@ -2928,37 +2936,37 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>tools</t>
+          <t>inference-frameworks</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>nuclear</t>
+          <t>llama-cpp</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>nuclear</t>
+          <t>llama.cpp</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Open-source music player and media utility application</t>
+          <t>C/C++ inference runtime for LLMs with efficient local deployment</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>https://github.com/nukeop/nuclear</t>
+          <t>https://github.com/ggml-org/llama.cpp</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>tool, desktop, media</t>
+          <t>inference, ggml, local-llm</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-8194-8006-f3252ec7f259</t>
+          <t>300d0e79-ce27-810a-a73f-f448ec025433</t>
         </is>
       </c>
       <c r="H55" t="n">
@@ -2973,36 +2981,36 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>next-ai-draw-io</t>
+          <t>aionui</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>next-ai-draw-io</t>
+          <t>AionUi</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>AI-assisted diagramming and flowchart generation tool</t>
+          <t>AI productivity UI toolset and utility platform</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>https://github.com/DayuanJiang/next-ai-draw-io</t>
+          <t>https://github.com/iOfficeAI/AionUi</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>tool, diagram, ai</t>
+          <t>tool, ui, productivity</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-812a-ad40-cf8897b1f4b1</t>
+          <t>300d0e79-ce27-81cf-b14e-c7dcf8b06178</t>
         </is>
       </c>
       <c r="H56" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -3013,36 +3021,36 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>antigravityquotawatcher</t>
+          <t>pastemd</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>AntigravityQuotaWatcher</t>
+          <t>PasteMD</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Quota monitoring and alerting utility for Antigravity services</t>
+          <t>Tool for converting and managing pasted content into Markdown</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>https://github.com/wusimpl/AntigravityQuotaWatcher</t>
+          <t>https://github.com/RICHQAQ/PasteMD</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>tool, monitoring, quota</t>
+          <t>tool, markdown, productivity</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-81a1-bee3-c615d19fe26b</t>
+          <t>300d0e79-ce27-8148-8215-d41868298788</t>
         </is>
       </c>
       <c r="H57" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -3053,28 +3061,36 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>openclaw</t>
+          <t>nuclear</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>openclaw</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr"/>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Open-source music player and media utility application</t>
+        </is>
+      </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>https://github.com/openclaw/openclaw</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr"/>
+          <t>https://github.com/nukeop/nuclear</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>tool, desktop, media</t>
+        </is>
+      </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>302d0e79-ce27-81e0-ace0-cafc375e8389</t>
+          <t>300d0e79-ce27-8194-8006-f3252ec7f259</t>
         </is>
       </c>
       <c r="H58" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59">
@@ -3085,136 +3101,144 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>learn-claude-code</t>
+          <t>next-ai-draw-io</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>learn-claude-code</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr"/>
+          <t>next-ai-draw-io</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>AI-assisted diagramming and flowchart generation tool</t>
+        </is>
+      </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>https://github.com/shareAI-lab/learn-claude-code</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr"/>
+          <t>https://github.com/DayuanJiang/next-ai-draw-io</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>tool, diagram, ai</t>
+        </is>
+      </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>302d0e79-ce27-8126-9a14-d1d622e92a41</t>
+          <t>300d0e79-ce27-812a-ad40-cf8897b1f4b1</t>
         </is>
       </c>
       <c r="H59" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>rag</t>
+          <t>tools</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>code-graph-rag</t>
+          <t>antigravityquotawatcher</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>code-graph-rag</t>
+          <t>AntigravityQuotaWatcher</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Graph-based retrieval-augmented generation for code understanding</t>
+          <t>Quota monitoring and alerting utility for Antigravity services</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>https://github.com/vitali87/code-graph-rag</t>
+          <t>https://github.com/wusimpl/AntigravityQuotaWatcher</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>rag, code, graph</t>
+          <t>tool, monitoring, quota</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>300d0e79-ce27-81a4-8bb7-d6eb9347ef22</t>
+          <t>300d0e79-ce27-81a1-bee3-c615d19fe26b</t>
         </is>
       </c>
       <c r="H60" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>rag</t>
+          <t>tools</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>deepwiki-open</t>
+          <t>learn-claude-code</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>deepwiki-open</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>Open-source DeepWiki-style project for codebase analysis and understanding</t>
-        </is>
-      </c>
+          <t>learn-claude-code</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr">
         <is>
-          <t>https://github.com/AsyncFuncAI/deepwiki-open</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>rag, code, analysis</t>
-        </is>
-      </c>
+          <t>https://github.com/shareAI-lab/learn-claude-code</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr">
         <is>
-          <t>301d0e79-ce27-818f-9977-cb06f3d39858</t>
+          <t>302d0e79-ce27-8126-9a14-d1d622e92a41</t>
         </is>
       </c>
       <c r="H61" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>voice</t>
+          <t>rag</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>gpt-sovits</t>
+          <t>code-graph-rag</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>GPT-SoVITS</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr"/>
+          <t>code-graph-rag</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Graph-based retrieval-augmented generation for code understanding</t>
+        </is>
+      </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>https://github.com/RVC-Boss/GPT-SoVITS</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr"/>
+          <t>https://github.com/vitali87/code-graph-rag</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>rag, code, graph</t>
+        </is>
+      </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>302d0e79-ce27-8176-8c62-f3b9f46ade9f</t>
+          <t>300d0e79-ce27-81a4-8bb7-d6eb9347ef22</t>
         </is>
       </c>
       <c r="H62" t="n">
@@ -3224,29 +3248,37 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>voice</t>
+          <t>rag</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>bark-voice-cloning</t>
+          <t>deepwiki-open</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Bark-Voice-Cloning</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr"/>
+          <t>deepwiki-open</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Open-source DeepWiki-style project for codebase analysis and understanding</t>
+        </is>
+      </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>https://github.com/KevinWang676/Bark-Voice-Cloning</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr"/>
+          <t>https://github.com/AsyncFuncAI/deepwiki-open</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>rag, code, analysis</t>
+        </is>
+      </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>302d0e79-ce27-816b-ad7b-db0165396bc3</t>
+          <t>304d0e79-ce27-8157-8c11-e49a06d03bd5</t>
         </is>
       </c>
       <c r="H63" t="n">
@@ -3261,28 +3293,28 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>retrieval-based-voice-conversion-webui</t>
+          <t>gpt-sovits</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Retrieval-based-Voice-Conversion-WebUI</t>
+          <t>GPT-SoVITS</t>
         </is>
       </c>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr">
         <is>
-          <t>https://github.com/RVC-Project/Retrieval-based-Voice-Conversion-WebUI</t>
+          <t>https://github.com/RVC-Boss/GPT-SoVITS</t>
         </is>
       </c>
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr">
         <is>
-          <t>302d0e79-ce27-8149-bdab-e74db6476b81</t>
+          <t>302d0e79-ce27-8176-8c62-f3b9f46ade9f</t>
         </is>
       </c>
       <c r="H64" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -3293,28 +3325,28 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>sensevoice</t>
+          <t>bark-voice-cloning</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>SenseVoice</t>
+          <t>Bark-Voice-Cloning</t>
         </is>
       </c>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr">
         <is>
-          <t>https://github.com/FunAudioLLM/SenseVoice</t>
+          <t>https://github.com/KevinWang676/Bark-Voice-Cloning</t>
         </is>
       </c>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr">
         <is>
-          <t>302d0e79-ce27-818e-ac17-f3d65c348cfb</t>
+          <t>302d0e79-ce27-816b-ad7b-db0165396bc3</t>
         </is>
       </c>
       <c r="H65" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -3325,28 +3357,28 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>cosyvoice</t>
+          <t>retrieval-based-voice-conversion-webui</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>CosyVoice</t>
+          <t>Retrieval-based-Voice-Conversion-WebUI</t>
         </is>
       </c>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr">
         <is>
-          <t>https://github.com/FunAudioLLM/CosyVoice</t>
+          <t>https://github.com/RVC-Project/Retrieval-based-Voice-Conversion-WebUI</t>
         </is>
       </c>
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr">
         <is>
-          <t>302d0e79-ce27-8146-8143-e0885ff719ad</t>
+          <t>302d0e79-ce27-8149-bdab-e74db6476b81</t>
         </is>
       </c>
       <c r="H66" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67">
@@ -3357,28 +3389,28 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>funasr</t>
+          <t>sensevoice</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>FunASR</t>
+          <t>SenseVoice</t>
         </is>
       </c>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr">
         <is>
-          <t>https://github.com/modelscope/FunASR</t>
+          <t>https://github.com/FunAudioLLM/SenseVoice</t>
         </is>
       </c>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr">
         <is>
-          <t>302d0e79-ce27-81ed-93d7-d112c9e49132</t>
+          <t>302d0e79-ce27-818e-ac17-f3d65c348cfb</t>
         </is>
       </c>
       <c r="H67" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68">
@@ -3389,28 +3421,420 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>fish-speech</t>
+          <t>cosyvoice</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>fish-speech</t>
+          <t>CosyVoice</t>
         </is>
       </c>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr">
         <is>
-          <t>https://github.com/fishaudio/fish-speech</t>
+          <t>https://github.com/FunAudioLLM/CosyVoice</t>
         </is>
       </c>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr">
         <is>
+          <t>302d0e79-ce27-8146-8143-e0885ff719ad</t>
+        </is>
+      </c>
+      <c r="H68" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>voice</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>funasr</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>FunASR</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr"/>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>https://github.com/modelscope/FunASR</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>302d0e79-ce27-81ed-93d7-d112c9e49132</t>
+        </is>
+      </c>
+      <c r="H69" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>voice</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>fish-speech</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>fish-speech</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr"/>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>https://github.com/fishaudio/fish-speech</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr">
+        <is>
           <t>302d0e79-ce27-8147-964d-eb843d564959</t>
         </is>
       </c>
-      <c r="H68" t="n">
+      <c r="H70" t="n">
         <v>6</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>voice</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>speech_recognition</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>speech_recognition</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr"/>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>https://github.com/Uberi/speech_recognition</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>304d0e79-ce27-8186-80cc-e784b94e0ccb</t>
+        </is>
+      </c>
+      <c r="H71" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>voice</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>voiceprintrecognition-pytorch</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>VoiceprintRecognition-Pytorch</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr"/>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>https://github.com/yeyupiaoling/VoiceprintRecognition-Pytorch</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>304d0e79-ce27-816d-b568-db84994a8ab9</t>
+        </is>
+      </c>
+      <c r="H72" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>route</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>litellm</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>litellm</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr"/>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>https://github.com/BerriAI/litellm</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>304d0e79-ce27-813a-8ecf-c48a57ab6811</t>
+        </is>
+      </c>
+      <c r="H73" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>route</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>claude-code-proxy</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>claude-code-proxy</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr"/>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>https://github.com/1rgs/claude-code-proxy</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>304d0e79-ce27-81d8-ab16-da52bf68b80d</t>
+        </is>
+      </c>
+      <c r="H74" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>route</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>fuergaosi233-claude-code-proxy</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>claude-code-proxy</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr"/>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>https://github.com/fuergaosi233/claude-code-proxy</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>304d0e79-ce27-81c1-9886-ef8e85208951</t>
+        </is>
+      </c>
+      <c r="H75" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>route</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>claude-code-router</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>claude-code-router</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr"/>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>https://github.com/musistudio/claude-code-router</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr"/>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>304d0e79-ce27-81ae-8888-d8509f12e8f9</t>
+        </is>
+      </c>
+      <c r="H76" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>桌面工具</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>anything-llm</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>anything-llm</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr"/>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>https://github.com/Mintplex-Labs/anything-llm</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr"/>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>304d0e79-ce27-8128-a4af-f969fcc69e40</t>
+        </is>
+      </c>
+      <c r="H77" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>桌面工具</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>nanobot</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>nanobot</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Lightweight AI agent framework and tooling</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>https://github.com/HKUDS/nanobot</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>ai, agents, framework</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>300d0e79-ce27-81fa-ad3e-f6cb074f1dc7</t>
+        </is>
+      </c>
+      <c r="H78" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>桌面工具</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>openclaw</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>openclaw</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr"/>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>https://github.com/openclaw/openclaw</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr"/>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>302d0e79-ce27-81e0-ace0-cafc375e8389</t>
+        </is>
+      </c>
+      <c r="H79" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>桌面工具</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>nanoclaw</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>nanoclaw</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr"/>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>https://github.com/qwibitai/nanoclaw</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>304d0e79-ce27-819c-bcc6-c595f337fc79</t>
+        </is>
+      </c>
+      <c r="H80" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>